<commit_message>
Updated figures and included new code for quantifying virospores for Magalie revisions
</commit_message>
<xml_diff>
--- a/Magalie_virospore_quant/Data/Annulus_Quant/20250317_virospore_multiquant_magalie.xlsx
+++ b/Magalie_virospore_quant/Data/Annulus_Quant/20250317_virospore_multiquant_magalie.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joyobrien/GitHub/VirosporeQuant/Magalie_virospore_quant/Data/Annulus_Quant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D472175D-53F0-924B-A0BB-1483D6D7E32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC775CA-F5D2-464D-8554-83220EC18296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="760" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{582F8197-BA5D-0947-BAA7-5525BF383706}"/>
+    <workbookView xWindow="2200" yWindow="760" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{582F8197-BA5D-0947-BAA7-5525BF383706}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="raw_data" sheetId="2" r:id="rId2"/>
-    <sheet name="raw_data_calculation" sheetId="3" r:id="rId3"/>
+    <sheet name="raw_data_joy" sheetId="4" r:id="rId3"/>
+    <sheet name="raw_data_calculation" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
   <si>
     <t>Plaque</t>
   </si>
@@ -578,15 +579,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C79FCC2-9D9F-C14A-9FDA-530344FAE2C8}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView zoomScale="106" workbookViewId="0">
+      <selection sqref="A1:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.83203125" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
     <col min="7" max="7" width="14.83203125" customWidth="1"/>
     <col min="8" max="9" width="25.83203125" customWidth="1"/>
     <col min="10" max="10" width="24.33203125" customWidth="1"/>
@@ -908,6 +909,250 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1B6F5F-45C7-9947-A7F2-60C7D5E2BB48}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0.2</v>
+      </c>
+      <c r="C2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>23</v>
+      </c>
+      <c r="F2">
+        <v>54</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.05</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+      <c r="C3">
+        <v>1.2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>42</v>
+      </c>
+      <c r="F3">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.05</v>
+      </c>
+      <c r="J3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>2.1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>292</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0.05</v>
+      </c>
+      <c r="I4">
+        <v>0.1</v>
+      </c>
+      <c r="J4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.2</v>
+      </c>
+      <c r="C5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>602</v>
+      </c>
+      <c r="F5">
+        <v>28</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0.05</v>
+      </c>
+      <c r="I5">
+        <v>0.1</v>
+      </c>
+      <c r="J5">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0.2</v>
+      </c>
+      <c r="C6">
+        <v>3.1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>29</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>0.1</v>
+      </c>
+      <c r="I6">
+        <v>0.2</v>
+      </c>
+      <c r="J6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0.2</v>
+      </c>
+      <c r="C7">
+        <v>3.2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>77</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>0.1</v>
+      </c>
+      <c r="I7">
+        <v>0.2</v>
+      </c>
+      <c r="J7">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E7F38B-5B73-0E4E-BA02-CB2C43BA0443}">
   <dimension ref="A1:L12"/>
   <sheetViews>

</xml_diff>